<commit_message>
almost done - some cleaning to do
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -192,7 +192,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -212,7 +212,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>regresion</a:t>
+              <a:t>ft_linear_regresion</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -220,7 +220,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="0">
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -289,7 +289,7 @@
             <c:dLbl>
               <c:idx val="10"/>
               <c:txPr>
-                <a:bodyPr wrap="none"/>
+                <a:bodyPr/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
@@ -310,7 +310,7 @@
             <c:dLbl>
               <c:idx val="19"/>
               <c:txPr>
-                <a:bodyPr wrap="none"/>
+                <a:bodyPr/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
@@ -329,7 +329,7 @@
               <c:separator> </c:separator>
             </c:dLbl>
             <c:txPr>
-              <a:bodyPr wrap="none"/>
+              <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -346,16 +346,11 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln w="0">
+              <a:ln>
                 <a:solidFill>
                   <a:srgbClr val="004586"/>
                 </a:solidFill>
@@ -531,11 +526,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="20190792"/>
-        <c:axId val="106526"/>
+        <c:axId val="70274675"/>
+        <c:axId val="8605899"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20190792"/>
+        <c:axId val="70274675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +551,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>milege</a:t>
+                  <a:t>mileage</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -564,7 +559,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln w="0">
+            <a:ln>
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -574,7 +569,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln>
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -591,12 +586,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106526"/>
+        <c:crossAx val="8605899"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106526"/>
+        <c:axId val="8605899"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +599,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="0">
+            <a:ln>
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -634,7 +629,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln w="0">
+            <a:ln>
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -644,7 +639,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln>
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -661,13 +656,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20190792"/>
+        <c:crossAx val="70274675"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="0">
+        <a:ln>
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -679,7 +674,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln w="0">
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -702,7 +697,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln w="0">
+    <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -714,15 +709,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:colOff>210240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>744120</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>119520</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>93960</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -730,8 +725,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1757160" y="667440"/>
-        <a:ext cx="6397920" cy="3678480"/>
+        <a:off x="1923840" y="492840"/>
+        <a:ext cx="6406560" cy="3678120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -751,11 +746,11 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.39"/>
@@ -964,10 +959,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>